<commit_message>
Update tabel Session di Excel
</commit_message>
<xml_diff>
--- a/AI Tugas Ver 2/Attendance.xlsx
+++ b/AI Tugas Ver 2/Attendance.xlsx
@@ -1,76 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ardian\Documents\BINUS\Artificial Intelligence\Tugas Akhir\AI Tugas Ver 2\AI Tugas Ver 2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Checkin" sheetId="1" r:id="rId1"/>
-    <sheet name="Checkout" sheetId="4" r:id="rId2"/>
-    <sheet name="Namelist" sheetId="3" r:id="rId3"/>
+    <sheet name="Checkin" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Checkout" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Namelist" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
-  <si>
-    <t>Check-In Record</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Check-Out Record</t>
-  </si>
-  <si>
-    <t>Name List</t>
-  </si>
-  <si>
-    <t>Agustinus Ardian C</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -88,31 +57,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,40 +441,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="53.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="3" customWidth="1"/>
+    <col width="53.44140625" customWidth="1" style="5" min="2" max="2"/>
+    <col width="17.5546875" customWidth="1" style="5" min="3" max="3"/>
+    <col width="17.77734375" customWidth="1" style="5" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Check-In Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+      <c r="B3">
+        <f>VLOOKUP(A3,'Namelist'!A:B,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>44575</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>09:08:01</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -457,39 +514,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="53.33203125" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" customWidth="1"/>
+    <col width="53.33203125" customWidth="1" style="5" min="2" max="2"/>
+    <col width="17.6640625" customWidth="1" style="5" min="3" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Check-Out Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+      <c r="B3">
+        <f>VLOOKUP(A3,'Namelist'!A:B,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>44575</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20:57:11</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -501,38 +586,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="53.33203125" style="3" customWidth="1"/>
+    <col width="53.33203125" customWidth="1" style="5" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Name List</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Agustinus Ardian C</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>